<commit_message>
Fix some events, fix pannel display when entering a region, fix some encounters.
</commit_message>
<xml_diff>
--- a/Obsidian/Game.xlsx
+++ b/Obsidian/Game.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Forêt d'Amaryllis" sheetId="4" r:id="rId3"/>
     <sheet name="Silverbridge" sheetId="7" r:id="rId4"/>
     <sheet name="Road 101" sheetId="8" r:id="rId5"/>
+    <sheet name="Ile inconnue" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="87">
   <si>
     <t>Pokémons</t>
   </si>
@@ -262,13 +263,40 @@
   </si>
   <si>
     <t>Huile</t>
+  </si>
+  <si>
+    <t>Monorpale</t>
+  </si>
+  <si>
+    <t>ETANG</t>
+  </si>
+  <si>
+    <t>OCEAN</t>
+  </si>
+  <si>
+    <t>GROTTE</t>
+  </si>
+  <si>
+    <t>Nosferapti</t>
+  </si>
+  <si>
+    <t>Taupiqueur</t>
+  </si>
+  <si>
+    <t>Machoc</t>
+  </si>
+  <si>
+    <t>Racaillou</t>
+  </si>
+  <si>
+    <t>Pierre Lune</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +330,14 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -376,7 +412,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -408,6 +444,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60 % - Accent1" xfId="2" builtinId="32"/>
@@ -417,7 +454,51 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Sortie" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="84">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -652,7 +733,220 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau21317" displayName="Tableau21317" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau21317" displayName="Tableau21317" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="83">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="82"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="81"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="80"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau414" displayName="Tableau414" ref="D3:F30" totalsRowShown="0" dataDxfId="51">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="50"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="49"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="48"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau615" displayName="Tableau615" ref="G3:G30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau716" displayName="Tableau716" ref="H3:I30" totalsRowShown="0" dataDxfId="44">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="43"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tableau2131725" displayName="Tableau2131725" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="41">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="40"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="39"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tableau4141826" displayName="Tableau4141826" ref="D3:F30" totalsRowShown="0" dataDxfId="37">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="36"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="35"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tableau6151927" displayName="Tableau6151927" ref="G3:G30" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tableau7162028" displayName="Tableau7162028" ref="H3:I30" totalsRowShown="0" dataDxfId="30">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="29"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tableau2131729" displayName="Tableau2131729" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="27">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="26"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="25"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tableau4141830" displayName="Tableau4141830" ref="D3:F30" totalsRowShown="0" dataDxfId="23">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="22"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="21"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tableau6151931" displayName="Tableau6151931" ref="G3:G30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau41418" displayName="Tableau41418" ref="D3:F30" totalsRowShown="0" dataDxfId="79">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="78"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="77"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="76"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tableau7162032" displayName="Tableau7162032" ref="H3:I30" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="15"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau21317292" displayName="Tableau21317292" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="13">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="12"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="11"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau41418303" displayName="Tableau41418303" ref="D3:F30" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="8"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="7"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau61519314" displayName="Tableau61519314" ref="G3:G30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau71620325" displayName="Tableau71620325" ref="H3:I30" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="1"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau61519" displayName="Tableau61519" ref="G3:G30" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="73"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau71620" displayName="Tableau71620" ref="H3:I30" totalsRowShown="0" dataDxfId="72">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="71"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau2131721" displayName="Tableau2131721" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="69">
   <autoFilter ref="A3:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Nom" dataDxfId="68"/>
@@ -663,120 +957,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau414" displayName="Tableau414" ref="D3:F30" totalsRowShown="0" dataDxfId="37">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="36"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="35"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="34"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau615" displayName="Tableau615" ref="G3:G30" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="31"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau716" displayName="Tableau716" ref="H3:I30" totalsRowShown="0" dataDxfId="30">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="29"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tableau2131725" displayName="Tableau2131725" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="26"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="25"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tableau4141826" displayName="Tableau4141826" ref="D3:F30" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="22"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="21"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="20"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tableau6151927" displayName="Tableau6151927" ref="G3:G30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="17"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tableau7162028" displayName="Tableau7162028" ref="H3:I30" totalsRowShown="0" dataDxfId="16">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="15"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tableau2131729" displayName="Tableau2131729" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="12"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="11"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tableau4141830" displayName="Tableau4141830" ref="D3:F30" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="8"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="7"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tableau6151931" displayName="Tableau6151931" ref="G3:G30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau41418" displayName="Tableau41418" ref="D3:F30" totalsRowShown="0" dataDxfId="65">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau4141822" displayName="Tableau4141822" ref="D3:F30" totalsRowShown="0" dataDxfId="65">
   <autoFilter ref="D3:F30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Pokémons" dataDxfId="64"/>
@@ -787,19 +969,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tableau7162032" displayName="Tableau7162032" ref="H3:I30" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="1"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau61519" displayName="Tableau61519" ref="G3:G30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau6151923" displayName="Tableau6151923" ref="G3:G30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="G3:G30"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nom" dataDxfId="59"/>
@@ -808,8 +979,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau71620" displayName="Tableau71620" ref="H3:I30" totalsRowShown="0" dataDxfId="58">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau7162024" displayName="Tableau7162024" ref="H3:I30" totalsRowShown="0" dataDxfId="58">
   <autoFilter ref="H3:I30"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nom" dataDxfId="57"/>
@@ -819,58 +990,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau2131721" displayName="Tableau2131721" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="55">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau213" displayName="Tableau213" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="55">
   <autoFilter ref="A3:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Nom" dataDxfId="54"/>
     <tableColumn id="2" name="Pokémons" dataDxfId="53"/>
     <tableColumn id="3" name="Niveaux" dataDxfId="52"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau4141822" displayName="Tableau4141822" ref="D3:F30" totalsRowShown="0" dataDxfId="51">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="50"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="49"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="48"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau6151923" displayName="Tableau6151923" ref="G3:G30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="45"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau7162024" displayName="Tableau7162024" ref="H3:I30" totalsRowShown="0" dataDxfId="44">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="43"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau213" displayName="Tableau213" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="41">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="40"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="39"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1915,7 +2041,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,9 +2185,24 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8">
+        <v>9</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="8">
+        <v>10</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2149,6 +2290,437 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="8">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="8">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="8">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="8">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="8">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="8">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="8">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="8">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="8">
+        <v>11</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="8">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="13"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -2229,72 +2801,44 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="D4" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I4" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="8">
-        <v>10</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="E5" s="3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="8">
-        <v>10</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E6" s="3">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>77</v>
@@ -2304,17 +2848,11 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="8">
-        <v>10</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="E7" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>58</v>
@@ -2322,236 +2860,87 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="E8" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="8">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="8">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="8">
-        <v>11</v>
-      </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="8">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="8">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="8">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="8">
-        <v>11</v>
-      </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="8">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="8">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="13"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish scripting on Island of Road 101
</commit_message>
<xml_diff>
--- a/Obsidian/Game.xlsx
+++ b/Obsidian/Game.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Silverbridge" sheetId="7" r:id="rId4"/>
     <sheet name="Road 101" sheetId="8" r:id="rId5"/>
     <sheet name="Ile inconnue" sheetId="9" r:id="rId6"/>
+    <sheet name="Fusiville" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="108">
   <si>
     <t>Pokémons</t>
   </si>
@@ -296,6 +297,63 @@
   </si>
   <si>
     <t>PV Plus</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Scarhino</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Volcaropod</t>
+  </si>
+  <si>
+    <t>Kraknoix</t>
+  </si>
+  <si>
+    <t>Reptincel</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>Abo</t>
+  </si>
+  <si>
+    <t>Nidoran♀</t>
+  </si>
+  <si>
+    <t>Nidoran♂</t>
+  </si>
+  <si>
+    <t>Luc</t>
+  </si>
+  <si>
+    <t>Rondoudou</t>
+  </si>
+  <si>
+    <t>Tarsal</t>
+  </si>
+  <si>
+    <t>Mélofée</t>
+  </si>
+  <si>
+    <t>Le mari perdu</t>
+  </si>
+  <si>
+    <t>Une Accréditation difficile à obtenir</t>
+  </si>
+  <si>
+    <t>Super Bonbon</t>
+  </si>
+  <si>
+    <t>NORTH SEA</t>
+  </si>
+  <si>
+    <t>Repousse</t>
   </si>
 </sst>
 </file>
@@ -460,7 +518,51 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Sortie" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="98">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -739,7 +841,265 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau21317" displayName="Tableau21317" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau21317" displayName="Tableau21317" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="97">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="96"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="95"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="94"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau414" displayName="Tableau414" ref="D3:F30" totalsRowShown="0" dataDxfId="65">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="64"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="63"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="62"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau615" displayName="Tableau615" ref="G3:G30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="59"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau716" displayName="Tableau716" ref="H3:I30" totalsRowShown="0" dataDxfId="58">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="57"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tableau2131725" displayName="Tableau2131725" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="55">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="54"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="53"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="52"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tableau4141826" displayName="Tableau4141826" ref="D3:F30" totalsRowShown="0" dataDxfId="51">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="50"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="49"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="48"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tableau6151927" displayName="Tableau6151927" ref="G3:G30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tableau7162028" displayName="Tableau7162028" ref="H3:I30" totalsRowShown="0" dataDxfId="44">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="43"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tableau2131729" displayName="Tableau2131729" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="41">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="40"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="39"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tableau4141830" displayName="Tableau4141830" ref="D3:F30" totalsRowShown="0" dataDxfId="37">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="36"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="35"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tableau6151931" displayName="Tableau6151931" ref="G3:G30" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau41418" displayName="Tableau41418" ref="D3:F30" totalsRowShown="0" dataDxfId="93">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="92"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="91"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="90"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tableau7162032" displayName="Tableau7162032" ref="H3:I30" totalsRowShown="0" dataDxfId="30">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="29"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau21317292" displayName="Tableau21317292" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="27">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="26"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="25"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau41418303" displayName="Tableau41418303" ref="D3:F30" totalsRowShown="0" dataDxfId="23">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="22"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="21"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau61519314" displayName="Tableau61519314" ref="G3:G30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau71620325" displayName="Tableau71620325" ref="H3:I30" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="15"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau213172926" displayName="Tableau213172926" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="13">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="12"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="11"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau414183037" displayName="Tableau414183037" ref="D3:F30" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="8"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="7"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau615193148" displayName="Tableau615193148" ref="G3:G30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau716203259" displayName="Tableau716203259" ref="H3:I30" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="1"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau61519" displayName="Tableau61519" ref="G3:G30" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="87"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau71620" displayName="Tableau71620" ref="H3:I30" totalsRowShown="0" dataDxfId="86">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="85"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="84"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau2131721" displayName="Tableau2131721" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="83">
   <autoFilter ref="A3:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Nom" dataDxfId="82"/>
@@ -750,120 +1110,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau414" displayName="Tableau414" ref="D3:F30" totalsRowShown="0" dataDxfId="51">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="50"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="49"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="48"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau615" displayName="Tableau615" ref="G3:G30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="45"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau716" displayName="Tableau716" ref="H3:I30" totalsRowShown="0" dataDxfId="44">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="43"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tableau2131725" displayName="Tableau2131725" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="41">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="40"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="39"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="38"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tableau4141826" displayName="Tableau4141826" ref="D3:F30" totalsRowShown="0" dataDxfId="37">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="36"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="35"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="34"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tableau6151927" displayName="Tableau6151927" ref="G3:G30" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="31"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tableau7162028" displayName="Tableau7162028" ref="H3:I30" totalsRowShown="0" dataDxfId="30">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="29"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tableau2131729" displayName="Tableau2131729" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="26"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="25"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tableau4141830" displayName="Tableau4141830" ref="D3:F30" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="22"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="21"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="20"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tableau6151931" displayName="Tableau6151931" ref="G3:G30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="17"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau41418" displayName="Tableau41418" ref="D3:F30" totalsRowShown="0" dataDxfId="79">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau4141822" displayName="Tableau4141822" ref="D3:F30" totalsRowShown="0" dataDxfId="79">
   <autoFilter ref="D3:F30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Pokémons" dataDxfId="78"/>
@@ -874,64 +1122,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tableau7162032" displayName="Tableau7162032" ref="H3:I30" totalsRowShown="0" dataDxfId="16">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="15"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau21317292" displayName="Tableau21317292" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="12"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="11"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau41418303" displayName="Tableau41418303" ref="D3:F30" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="8"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="7"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau61519314" displayName="Tableau61519314" ref="G3:G30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau71620325" displayName="Tableau71620325" ref="H3:I30" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="1"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau61519" displayName="Tableau61519" ref="G3:G30" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau6151923" displayName="Tableau6151923" ref="G3:G30" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="G3:G30"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nom" dataDxfId="73"/>
@@ -940,8 +1132,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau71620" displayName="Tableau71620" ref="H3:I30" totalsRowShown="0" dataDxfId="72">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau7162024" displayName="Tableau7162024" ref="H3:I30" totalsRowShown="0" dataDxfId="72">
   <autoFilter ref="H3:I30"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nom" dataDxfId="71"/>
@@ -951,58 +1143,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau2131721" displayName="Tableau2131721" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="69">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau213" displayName="Tableau213" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="69">
   <autoFilter ref="A3:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Nom" dataDxfId="68"/>
     <tableColumn id="2" name="Pokémons" dataDxfId="67"/>
     <tableColumn id="3" name="Niveaux" dataDxfId="66"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau4141822" displayName="Tableau4141822" ref="D3:F30" totalsRowShown="0" dataDxfId="65">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="64"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="63"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="62"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau6151923" displayName="Tableau6151923" ref="G3:G30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="59"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau7162024" displayName="Tableau7162024" ref="H3:I30" totalsRowShown="0" dataDxfId="58">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="57"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau213" displayName="Tableau213" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="55">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="54"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="53"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2299,7 +2446,700 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="8">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="8">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="8">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="8">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="8">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="8">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="8">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="8">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="8">
+        <v>11</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="8">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="9"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="9"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2377,74 +3217,51 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C4" s="8">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="3"/>
       <c r="G4" s="2" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="I4" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="8">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>56</v>
+      <c r="E5" s="3"/>
+      <c r="G5" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="I5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C6" s="8">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="H6" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="I6" s="8">
         <v>1</v>
@@ -2452,78 +3269,46 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C7" s="8">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="H7" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="B8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C9" s="8">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="8">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="C11" s="8">
         <v>11</v>
@@ -2531,434 +3316,107 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="B12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="8">
+        <v>11</v>
+      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="C13" s="8">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="C14" s="8">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="8">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C16" s="8">
         <v>11</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="8">
+        <v>12</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>74</v>
-      </c>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="C18" s="8">
-        <v>11</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="8">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="9"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="4">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="9"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing encounter tables. Small balancing.
</commit_message>
<xml_diff>
--- a/Obsidian/Game.xlsx
+++ b/Obsidian/Game.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Road 101" sheetId="8" r:id="rId5"/>
     <sheet name="Ile inconnue" sheetId="9" r:id="rId6"/>
     <sheet name="Fusiville" sheetId="11" r:id="rId7"/>
+    <sheet name="Road 102" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="112">
   <si>
     <t>Pokémons</t>
   </si>
@@ -354,6 +355,18 @@
   </si>
   <si>
     <t>Repousse</t>
+  </si>
+  <si>
+    <t>6-12</t>
+  </si>
+  <si>
+    <t>Piafabec</t>
+  </si>
+  <si>
+    <t>Granivol</t>
+  </si>
+  <si>
+    <t>Medhyèna</t>
   </si>
 </sst>
 </file>
@@ -518,7 +531,51 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Sortie" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="112">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -841,7 +898,310 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau21317" displayName="Tableau21317" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau21317" displayName="Tableau21317" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="111">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="110"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="109"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="108"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau414" displayName="Tableau414" ref="D3:F30" totalsRowShown="0" dataDxfId="79">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="78"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="77"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="76"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau615" displayName="Tableau615" ref="G3:G30" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="73"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau716" displayName="Tableau716" ref="H3:I30" totalsRowShown="0" dataDxfId="72">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="71"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tableau2131725" displayName="Tableau2131725" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="69">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="68"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="67"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="66"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tableau4141826" displayName="Tableau4141826" ref="D3:F30" totalsRowShown="0" dataDxfId="65">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="64"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="63"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="62"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tableau6151927" displayName="Tableau6151927" ref="G3:G30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="59"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tableau7162028" displayName="Tableau7162028" ref="H3:I30" totalsRowShown="0" dataDxfId="58">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="57"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tableau2131729" displayName="Tableau2131729" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="55">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="54"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="53"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="52"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tableau4141830" displayName="Tableau4141830" ref="D3:F30" totalsRowShown="0" dataDxfId="51">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="50"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="49"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="48"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tableau6151931" displayName="Tableau6151931" ref="G3:G30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau41418" displayName="Tableau41418" ref="D3:F30" totalsRowShown="0" dataDxfId="107">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="106"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="105"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="104"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tableau7162032" displayName="Tableau7162032" ref="H3:I30" totalsRowShown="0" dataDxfId="44">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="43"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau21317292" displayName="Tableau21317292" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="41">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="40"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="39"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau41418303" displayName="Tableau41418303" ref="D3:F30" totalsRowShown="0" dataDxfId="37">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="36"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="35"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau61519314" displayName="Tableau61519314" ref="G3:G30" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau71620325" displayName="Tableau71620325" ref="H3:I30" totalsRowShown="0" dataDxfId="30">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="29"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau213172926" displayName="Tableau213172926" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="27">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="26"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="25"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau414183037" displayName="Tableau414183037" ref="D3:F30" totalsRowShown="0" dataDxfId="23">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="22"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="21"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau615193148" displayName="Tableau615193148" ref="G3:G30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau716203259" displayName="Tableau716203259" ref="H3:I30" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="15"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau21317292610" displayName="Tableau21317292610" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="13">
+  <autoFilter ref="A3:C30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom" dataDxfId="12"/>
+    <tableColumn id="2" name="Pokémons" dataDxfId="11"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau61519" displayName="Tableau61519" ref="G3:G30" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="101"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau41418303711" displayName="Tableau41418303711" ref="D3:F30" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="D3:F30"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Pokémons" dataDxfId="8"/>
+    <tableColumn id="4" name="Pourcentage" dataDxfId="7"/>
+    <tableColumn id="3" name="Niveaux" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau61519314812" displayName="Tableau61519314812" ref="G3:G30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="G3:G30"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nom" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Tableau71620325933" displayName="Tableau71620325933" ref="H3:I30" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="1"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau71620" displayName="Tableau71620" ref="H3:I30" totalsRowShown="0" dataDxfId="100">
+  <autoFilter ref="H3:I30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nom" dataDxfId="99"/>
+    <tableColumn id="2" name="Quantité" dataDxfId="98"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau2131721" displayName="Tableau2131721" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="97">
   <autoFilter ref="A3:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Nom" dataDxfId="96"/>
@@ -852,120 +1212,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau414" displayName="Tableau414" ref="D3:F30" totalsRowShown="0" dataDxfId="65">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="64"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="63"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="62"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau615" displayName="Tableau615" ref="G3:G30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="59"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau716" displayName="Tableau716" ref="H3:I30" totalsRowShown="0" dataDxfId="58">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="57"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tableau2131725" displayName="Tableau2131725" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="55">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="54"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="53"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="52"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tableau4141826" displayName="Tableau4141826" ref="D3:F30" totalsRowShown="0" dataDxfId="51">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="50"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="49"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="48"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tableau6151927" displayName="Tableau6151927" ref="G3:G30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="45"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tableau7162028" displayName="Tableau7162028" ref="H3:I30" totalsRowShown="0" dataDxfId="44">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="43"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tableau2131729" displayName="Tableau2131729" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="41">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="40"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="39"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="38"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tableau4141830" displayName="Tableau4141830" ref="D3:F30" totalsRowShown="0" dataDxfId="37">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="36"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="35"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="34"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tableau6151931" displayName="Tableau6151931" ref="G3:G30" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="31"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tableau41418" displayName="Tableau41418" ref="D3:F30" totalsRowShown="0" dataDxfId="93">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau4141822" displayName="Tableau4141822" ref="D3:F30" totalsRowShown="0" dataDxfId="93">
   <autoFilter ref="D3:F30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Pokémons" dataDxfId="92"/>
@@ -976,109 +1224,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tableau7162032" displayName="Tableau7162032" ref="H3:I30" totalsRowShown="0" dataDxfId="30">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="29"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau21317292" displayName="Tableau21317292" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="26"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="25"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau41418303" displayName="Tableau41418303" ref="D3:F30" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="22"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="21"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="20"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau61519314" displayName="Tableau61519314" ref="G3:G30" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="17"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau71620325" displayName="Tableau71620325" ref="H3:I30" totalsRowShown="0" dataDxfId="16">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="15"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="14"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau213172926" displayName="Tableau213172926" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="13">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="12"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="11"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau414183037" displayName="Tableau414183037" ref="D3:F30" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="8"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="7"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau615193148" displayName="Tableau615193148" ref="G3:G30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau716203259" displayName="Tableau716203259" ref="H3:I30" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="1"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tableau61519" displayName="Tableau61519" ref="G3:G30" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau6151923" displayName="Tableau6151923" ref="G3:G30" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="G3:G30"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nom" dataDxfId="87"/>
@@ -1087,8 +1234,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tableau71620" displayName="Tableau71620" ref="H3:I30" totalsRowShown="0" dataDxfId="86">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau7162024" displayName="Tableau7162024" ref="H3:I30" totalsRowShown="0" dataDxfId="86">
   <autoFilter ref="H3:I30"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nom" dataDxfId="85"/>
@@ -1098,58 +1245,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tableau2131721" displayName="Tableau2131721" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="83">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau213" displayName="Tableau213" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="83">
   <autoFilter ref="A3:C30"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Nom" dataDxfId="82"/>
     <tableColumn id="2" name="Pokémons" dataDxfId="81"/>
     <tableColumn id="3" name="Niveaux" dataDxfId="80"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tableau4141822" displayName="Tableau4141822" ref="D3:F30" totalsRowShown="0" dataDxfId="79">
-  <autoFilter ref="D3:F30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Pokémons" dataDxfId="78"/>
-    <tableColumn id="4" name="Pourcentage" dataDxfId="77"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="76"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tableau6151923" displayName="Tableau6151923" ref="G3:G30" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
-  <autoFilter ref="G3:G30"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Nom" dataDxfId="73"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tableau7162024" displayName="Tableau7162024" ref="H3:I30" totalsRowShown="0" dataDxfId="72">
-  <autoFilter ref="H3:I30"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Nom" dataDxfId="71"/>
-    <tableColumn id="2" name="Quantité" dataDxfId="70"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tableau213" displayName="Tableau213" ref="A3:C30" insertRowShift="1" totalsRowShown="0" dataDxfId="69">
-  <autoFilter ref="A3:C30"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Nom" dataDxfId="68"/>
-    <tableColumn id="2" name="Pokémons" dataDxfId="67"/>
-    <tableColumn id="3" name="Niveaux" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2194,7 +2296,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2549,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,7 +2850,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C16" s="8">
         <v>11</v>
@@ -2893,7 +2995,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,23 +3149,65 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="9"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="3"/>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="3"/>
@@ -3139,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3225,7 +3369,9 @@
       <c r="C4" s="8">
         <v>15</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="G4" s="2" t="s">
         <v>103</v>
@@ -3238,7 +3384,15 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>104</v>
       </c>
@@ -3259,7 +3413,15 @@
       <c r="C6" s="8">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>38</v>
       </c>
@@ -3274,7 +3436,15 @@
       <c r="C7" s="8">
         <v>12</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>76</v>
       </c>
@@ -3289,7 +3459,15 @@
       <c r="C8" s="8">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -3298,7 +3476,15 @@
       <c r="C9" s="8">
         <v>14</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="3"/>
@@ -3435,4 +3621,245 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="9"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>